<commit_message>
Post Class Raw Update
</commit_message>
<xml_diff>
--- a/Sprint 1.xlsx
+++ b/Sprint 1.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="20490" windowHeight="7425"/>
+    <workbookView xWindow="0" yWindow="6000" windowWidth="20490" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="3" r:id="rId1"/>
+    <sheet name="Product Backlog" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Sprint 1'!$B$2:$X$26</definedName>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="97">
   <si>
     <t>Status</t>
   </si>
@@ -106,9 +107,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>1) Create the employee registration view within the solution</t>
-  </si>
-  <si>
     <t>3) Create the "Employee" table within the database</t>
   </si>
   <si>
@@ -116,9 +114,6 @@
   </si>
   <si>
     <t>Daycare Management System</t>
-  </si>
-  <si>
-    <t>1) Create the Login View within the Presentation Layer</t>
   </si>
   <si>
     <t>1) Create the parent registration view within the presentation layer</t>
@@ -143,12 +138,6 @@
     <t>3) Add "Child" tables within the database</t>
   </si>
   <si>
-    <t>5) Ensure register process has a loading and start page.</t>
-  </si>
-  <si>
-    <t>1) Create a view to display children information</t>
-  </si>
-  <si>
     <t>2) Code the Business layer methods to pull children information from the database</t>
   </si>
   <si>
@@ -159,6 +148,168 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Product Backlog</t>
+  </si>
+  <si>
+    <t>Parent Registers children for classes from home</t>
+  </si>
+  <si>
+    <t>Employees can leave notes for children that parents can view at home</t>
+  </si>
+  <si>
+    <t>Employees can send emails to a parent or a select group of parentts</t>
+  </si>
+  <si>
+    <t>Employees can generate reports that can be distributed to parents</t>
+  </si>
+  <si>
+    <t>Employees are able to check in a child</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Story points</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parents can leave notes for employees can view </t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Finished Testing</t>
+  </si>
+  <si>
+    <t>In Review</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Abadoned</t>
+  </si>
+  <si>
+    <t>Original Estimate: 21</t>
+  </si>
+  <si>
+    <t>Create first Solution</t>
+  </si>
+  <si>
+    <t>Upload to GitHub</t>
+  </si>
+  <si>
+    <t>Presentation Layer Design</t>
+  </si>
+  <si>
+    <t>UML Diagrams for Business Logic</t>
+  </si>
+  <si>
+    <t>Database Design</t>
+  </si>
+  <si>
+    <t>Create and Test database within Source Control</t>
+  </si>
+  <si>
+    <t>Kevin / Nick</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Stave</t>
+  </si>
+  <si>
+    <t>Create the default page for the site</t>
+  </si>
+  <si>
+    <t>1) Create the  Log in pop up within the Presentation Layer</t>
+  </si>
+  <si>
+    <t>Estimated: 13</t>
+  </si>
+  <si>
+    <t>As a / an website visitor, I want to be able to register a child to the company.</t>
+  </si>
+  <si>
+    <t>As a / an website visitor, I want to be able to view a registered child and view all information.</t>
+  </si>
+  <si>
+    <t>5) Test completed task</t>
+  </si>
+  <si>
+    <t>Actual: 10</t>
+  </si>
+  <si>
+    <t>Estimated: 5</t>
+  </si>
+  <si>
+    <t>1) Create the child view page within the presentation layer</t>
+  </si>
+  <si>
+    <t>3) Code the return stored procedures to pull children</t>
+  </si>
+  <si>
+    <t>5) Testing</t>
+  </si>
+  <si>
+    <t>Actua Estimate: 7</t>
+  </si>
+  <si>
+    <t>Estimate: 5</t>
+  </si>
+  <si>
+    <t>1) Create roles within the employees</t>
+  </si>
+  <si>
+    <t>2) Create a maintenance page for Admin levels</t>
+  </si>
+  <si>
+    <t>1) Create the employee registration view within the maintenance page</t>
+  </si>
+  <si>
+    <t>3) Create a default page that will allow employees to log in</t>
+  </si>
+  <si>
+    <t>Create the information page: Parents and Children</t>
+  </si>
+  <si>
+    <t>2) Code the business layer to pull parents then pull children based on parent</t>
+  </si>
+  <si>
+    <t>3) Create SPROCS to return information on parents and children</t>
+  </si>
+  <si>
+    <t>5) testing</t>
+  </si>
+  <si>
+    <t>1) Create a view to search all children information</t>
+  </si>
+  <si>
+    <t>3) Code the Sprocs to pull all children</t>
+  </si>
+  <si>
+    <t>4) testing</t>
   </si>
 </sst>
 </file>
@@ -169,7 +320,7 @@
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="165" formatCode="0_);\(0\)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -279,8 +430,44 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,8 +486,13 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -328,8 +520,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -338,8 +552,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -468,14 +683,92 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="3" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="16"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="43"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="58"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -766,53 +1059,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="16"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="43"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="58"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <color theme="1" tint="0.24994659260841701"/>
@@ -1041,7 +1287,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$G$39:$K$39</c:f>
+              <c:f>'Sprint 1'!$G$69:$K$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1074,11 +1320,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="227431648"/>
-        <c:axId val="227431088"/>
+        <c:axId val="3477872"/>
+        <c:axId val="217616016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="227431648"/>
+        <c:axId val="3477872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1366,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227431088"/>
+        <c:crossAx val="217616016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1128,7 +1374,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="227431088"/>
+        <c:axId val="217616016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,7 +1424,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227431648"/>
+        <c:crossAx val="3477872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1843,19 +2089,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B5:K39" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="B5:K39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B5:K69" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="B5:K69"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Product Backlog Item" dataDxfId="9"/>
-    <tableColumn id="5" name="Task" dataDxfId="8"/>
-    <tableColumn id="4" name="Volunteer" dataDxfId="7"/>
-    <tableColumn id="3" name="Status" dataDxfId="6"/>
-    <tableColumn id="2" name="Original Estimate" dataDxfId="5"/>
-    <tableColumn id="6" name="Week 1" dataDxfId="4"/>
-    <tableColumn id="7" name="Week 2" dataDxfId="3"/>
-    <tableColumn id="11" name="Week 3" dataDxfId="2"/>
-    <tableColumn id="8" name="Week 4" dataDxfId="1"/>
-    <tableColumn id="9" name="Sprint Review" dataDxfId="0"/>
+    <tableColumn id="1" name="Product Backlog Item" dataDxfId="13"/>
+    <tableColumn id="5" name="Task" dataDxfId="12"/>
+    <tableColumn id="4" name="Volunteer" dataDxfId="11"/>
+    <tableColumn id="3" name="Status" dataDxfId="10"/>
+    <tableColumn id="2" name="Original Estimate" dataDxfId="9"/>
+    <tableColumn id="6" name="Week 1" dataDxfId="8"/>
+    <tableColumn id="7" name="Week 2" dataDxfId="7"/>
+    <tableColumn id="11" name="Week 3" dataDxfId="6"/>
+    <tableColumn id="8" name="Week 4" dataDxfId="5"/>
+    <tableColumn id="9" name="Sprint Review" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Project Performance Report" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1864,42 +2110,42 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="ProjectPerformanceReport_colors">
+    <a:clrScheme name="Green">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="323232"/>
+        <a:srgbClr val="455F51"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="F0F9F9"/>
+        <a:srgbClr val="E3DED1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="00AFDB"/>
+        <a:srgbClr val="549E39"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="5E9732"/>
+        <a:srgbClr val="8AB833"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="B5121B"/>
+        <a:srgbClr val="C0CF3A"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="EC881D"/>
+        <a:srgbClr val="029676"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="6054A4"/>
+        <a:srgbClr val="4AB5C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="EBB304"/>
+        <a:srgbClr val="0989B1"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="00AFDB"/>
+        <a:srgbClr val="6B9F25"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="6054A4"/>
+        <a:srgbClr val="BA6906"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="ProjectPerformanceReport_fonts">
@@ -2092,10 +2338,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:X52"/>
+  <dimension ref="B2:X82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2121,7 +2367,7 @@
   <sheetData>
     <row r="2" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -2221,19 +2467,17 @@
     </row>
     <row r="6" spans="2:24" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="33" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>24</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E6" s="35"/>
       <c r="F6" s="35">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="G6" s="35">
         <v>0</v>
@@ -2266,18 +2510,18 @@
       <c r="W6" s="10"/>
     </row>
     <row r="7" spans="2:24" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="33"/>
+      <c r="B7" s="52" t="s">
+        <v>63</v>
+      </c>
       <c r="C7" s="33" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>24</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E7" s="35"/>
       <c r="F7" s="35">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G7" s="35" t="s">
         <v>28</v>
@@ -2311,16 +2555,14 @@
     <row r="8" spans="2:24" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="33"/>
       <c r="C8" s="33" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D8" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="35" t="s">
-        <v>24</v>
-      </c>
+      <c r="E8" s="35"/>
       <c r="F8" s="35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" s="35" t="s">
         <v>28</v>
@@ -2350,35 +2592,23 @@
       <c r="V8" s="27"/>
       <c r="W8" s="29"/>
     </row>
-    <row r="9" spans="2:24" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:24" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="33"/>
       <c r="C9" s="33" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>24</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E9" s="35"/>
       <c r="F9" s="35">
         <v>3</v>
       </c>
-      <c r="G9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="35" t="s">
-        <v>28</v>
-      </c>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
       <c r="L9" s="21"/>
       <c r="M9" s="20"/>
       <c r="N9" s="21"/>
@@ -2392,17 +2622,23 @@
       <c r="V9" s="15"/>
       <c r="W9" s="30"/>
     </row>
-    <row r="10" spans="2:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
+    <row r="10" spans="2:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35">
+        <v>3</v>
+      </c>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
       <c r="L10" s="21"/>
       <c r="M10" s="20"/>
       <c r="N10" s="21"/>
@@ -2416,37 +2652,23 @@
       <c r="V10" s="15"/>
       <c r="W10" s="30"/>
     </row>
-    <row r="11" spans="2:24" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="33" t="s">
-        <v>6</v>
-      </c>
+    <row r="11" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="33"/>
       <c r="C11" s="33" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>24</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E11" s="35"/>
       <c r="F11" s="35">
-        <v>5</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" s="35" t="s">
-        <v>28</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
       <c r="L11" s="21"/>
       <c r="M11" s="20"/>
       <c r="N11" s="21"/>
@@ -2463,32 +2685,20 @@
     <row r="12" spans="2:24" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="33"/>
       <c r="C12" s="33" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E12" s="35"/>
       <c r="F12" s="35">
-        <v>4</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K12" s="35" t="s">
-        <v>28</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
       <c r="L12" s="21"/>
       <c r="M12" s="20"/>
       <c r="N12" s="21"/>
@@ -2505,10 +2715,10 @@
     <row r="13" spans="2:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="33"/>
       <c r="C13" s="33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>24</v>
@@ -2516,21 +2726,11 @@
       <c r="F13" s="35">
         <v>3</v>
       </c>
-      <c r="G13" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K13" s="35" t="s">
-        <v>28</v>
-      </c>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
       <c r="L13" s="21"/>
       <c r="M13" s="20"/>
       <c r="N13" s="21"/>
@@ -2547,32 +2747,22 @@
     <row r="14" spans="2:24" s="3" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="33"/>
       <c r="C14" s="33" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="35">
-        <v>2</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K14" s="35" t="s">
-        <v>28</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
       <c r="L14" s="21"/>
       <c r="M14" s="20"/>
       <c r="N14" s="21"/>
@@ -2589,32 +2779,22 @@
     <row r="15" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="33"/>
       <c r="C15" s="33" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F15" s="35">
-        <v>1</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15" s="35" t="s">
-        <v>28</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
       <c r="L15" s="21"/>
       <c r="M15" s="20"/>
       <c r="N15" s="21"/>
@@ -2629,16 +2809,24 @@
       <c r="W15" s="30"/>
     </row>
     <row r="16" spans="2:24" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="35">
+        <v>3</v>
+      </c>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
       <c r="L16" s="20"/>
       <c r="M16" s="21"/>
       <c r="N16" s="20"/>
@@ -2653,36 +2841,16 @@
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="35">
-        <v>5</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K17" s="35" t="s">
-        <v>28</v>
-      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
       <c r="L17" s="21"/>
       <c r="M17" s="20"/>
       <c r="N17" s="21"/>
@@ -2698,33 +2866,15 @@
     </row>
     <row r="18" spans="2:23" s="3" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="33"/>
-      <c r="C18" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="35">
-        <v>4</v>
-      </c>
-      <c r="G18" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J18" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K18" s="35" t="s">
-        <v>28</v>
-      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
       <c r="L18" s="25"/>
       <c r="M18" s="26"/>
       <c r="N18" s="25"/>
@@ -2740,33 +2890,15 @@
     </row>
     <row r="19" spans="2:23" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="33"/>
-      <c r="C19" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="35">
-        <v>3</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K19" s="35" t="s">
-        <v>28</v>
-      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
       <c r="L19" s="21"/>
       <c r="M19" s="20"/>
       <c r="N19" s="21"/>
@@ -2782,33 +2914,15 @@
     </row>
     <row r="20" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="33"/>
-      <c r="C20" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="35">
-        <v>2</v>
-      </c>
-      <c r="G20" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K20" s="35" t="s">
-        <v>28</v>
-      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
       <c r="L20" s="21"/>
       <c r="M20" s="20"/>
       <c r="N20" s="21"/>
@@ -2823,16 +2937,16 @@
       <c r="W20" s="30"/>
     </row>
     <row r="21" spans="2:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
       <c r="L21" s="21"/>
       <c r="M21" s="20"/>
       <c r="N21" s="21"/>
@@ -2847,36 +2961,16 @@
       <c r="W21" s="30"/>
     </row>
     <row r="22" spans="2:23" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="35">
-        <v>5</v>
-      </c>
-      <c r="G22" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H22" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J22" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K22" s="35" t="s">
-        <v>28</v>
-      </c>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
       <c r="L22" s="21"/>
       <c r="M22" s="20"/>
       <c r="N22" s="21"/>
@@ -2891,19 +2985,11 @@
       <c r="W22" s="30"/>
     </row>
     <row r="23" spans="2:23" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="39"/>
-      <c r="C23" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="35">
-        <v>4</v>
-      </c>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
       <c r="G23" s="35" t="s">
         <v>28</v>
       </c>
@@ -2932,35 +3018,17 @@
       <c r="V23" s="15"/>
       <c r="W23" s="30"/>
     </row>
-    <row r="24" spans="2:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="39"/>
-      <c r="C24" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="35">
-        <v>3</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J24" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K24" s="35" t="s">
-        <v>28</v>
-      </c>
+    <row r="24" spans="2:23" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
       <c r="L24" s="21"/>
       <c r="M24" s="20"/>
       <c r="N24" s="21"/>
@@ -2974,13 +3042,15 @@
       <c r="V24" s="15"/>
       <c r="W24" s="30"/>
     </row>
-    <row r="25" spans="2:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="39"/>
+    <row r="25" spans="2:23" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="33" t="s">
+        <v>6</v>
+      </c>
       <c r="C25" s="33" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E25" s="35" t="s">
         <v>24</v>
@@ -3017,16 +3087,18 @@
       <c r="W25" s="30"/>
     </row>
     <row r="26" spans="2:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
+      <c r="B26" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="33"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
       <c r="L26" s="21"/>
       <c r="M26" s="20"/>
       <c r="N26" s="21"/>
@@ -3041,20 +3113,18 @@
       <c r="W26" s="30"/>
     </row>
     <row r="27" spans="2:23" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="39" t="s">
-        <v>14</v>
-      </c>
+      <c r="B27" s="33"/>
       <c r="C27" s="33" t="s">
         <v>33</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E27" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F27" s="35">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G27" s="35" t="s">
         <v>28</v>
@@ -3078,18 +3148,18 @@
       <c r="W27" s="1"/>
     </row>
     <row r="28" spans="2:23" ht="24" x14ac:dyDescent="0.2">
-      <c r="B28" s="39"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E28" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F28" s="35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G28" s="35" t="s">
         <v>28</v>
@@ -3112,19 +3182,19 @@
       <c r="V28" s="5"/>
       <c r="W28" s="1"/>
     </row>
-    <row r="29" spans="2:23" ht="24" x14ac:dyDescent="0.2">
-      <c r="B29" s="39"/>
+    <row r="29" spans="2:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B29" s="33"/>
       <c r="C29" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E29" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F29" s="35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29" s="35" t="s">
         <v>28</v>
@@ -3151,9 +3221,9 @@
       <c r="W29" s="1"/>
     </row>
     <row r="30" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="39"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="35" t="s">
         <v>22</v>
@@ -3186,66 +3256,68 @@
       <c r="W30" s="1"/>
     </row>
     <row r="31" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="33"/>
-      <c r="C31" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="35" t="s">
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+    </row>
+    <row r="32" spans="2:23" ht="24" x14ac:dyDescent="0.2">
+      <c r="B32" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="35">
+      <c r="F32" s="35">
         <v>2</v>
       </c>
-      <c r="G31" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="H31" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="J31" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K31" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="2:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
+      <c r="G32" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J32" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K32" s="35" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="33" spans="2:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="33" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E33" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F33" s="35">
-        <v>5</v>
-      </c>
-      <c r="G33" s="35">
         <v>3</v>
       </c>
+      <c r="G33" s="35" t="s">
+        <v>28</v>
+      </c>
       <c r="H33" s="35" t="s">
         <v>28</v>
       </c>
@@ -3260,21 +3332,23 @@
       </c>
     </row>
     <row r="34" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="33"/>
+      <c r="B34" s="33" t="s">
+        <v>79</v>
+      </c>
       <c r="C34" s="33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E34" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F34" s="35">
-        <v>4</v>
-      </c>
-      <c r="G34" s="35">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G34" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="H34" s="35" t="s">
         <v>28</v>
@@ -3291,327 +3365,947 @@
     </row>
     <row r="35" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="33"/>
-      <c r="C35" s="38" t="s">
-        <v>12</v>
+      <c r="C35" s="33" t="s">
+        <v>78</v>
       </c>
       <c r="D35" s="35" t="s">
         <v>22</v>
       </c>
       <c r="E35" s="35" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F35" s="35">
-        <f>SUM(F30,F25,F20,F15,F9)</f>
-        <v>10</v>
-      </c>
-      <c r="G35" s="35">
-        <f t="shared" ref="F35:K35" si="0">SUM(G30,G25,G15,G9,G20)</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K35" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G35" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J35" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" s="35" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="33"/>
-      <c r="C36" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="35">
-        <f>SUM(F34,F28,F23,F18,F12,F7)</f>
-        <v>25</v>
-      </c>
-      <c r="G36" s="35">
-        <f>SUM(G34,G28,G23,G18,G12,G7)</f>
-        <v>2</v>
-      </c>
-      <c r="H36" s="35">
-        <f>SUM(H34,H28,H23,H18,H12,H7)</f>
-        <v>0</v>
-      </c>
-      <c r="I36" s="35">
-        <f>SUM(I34,I28,I23,I18,I12,I7)</f>
-        <v>0</v>
-      </c>
-      <c r="J36" s="35">
-        <f>SUM(J34,J28,J23,J18,J12,J7)</f>
-        <v>0</v>
-      </c>
-      <c r="K36" s="35">
-        <f>SUM(K34,K28,K23,K18,K12,K7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="33"/>
-      <c r="C37" s="38" t="s">
-        <v>12</v>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="42"/>
+    </row>
+    <row r="37" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>81</v>
       </c>
       <c r="D37" s="35" t="s">
         <v>23</v>
       </c>
       <c r="E37" s="35" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F37" s="35">
-        <f>SUM(F33,F27,F22,F17,F11,F6)</f>
-        <v>28</v>
-      </c>
-      <c r="G37" s="35"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="35"/>
-    </row>
-    <row r="38" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="33"/>
-      <c r="C38" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="42"/>
+    </row>
+    <row r="38" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="35">
+        <v>2</v>
+      </c>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="42"/>
+    </row>
+    <row r="39" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="35">
+        <v>1</v>
+      </c>
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="42"/>
+    </row>
+    <row r="40" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="33"/>
+      <c r="C40" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="35">
+        <v>2</v>
+      </c>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42"/>
+    </row>
+    <row r="41" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
+      <c r="K41" s="42"/>
+    </row>
+    <row r="42" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="42"/>
+    </row>
+    <row r="43" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="42"/>
+    </row>
+    <row r="44" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
+      <c r="K44" s="42"/>
+    </row>
+    <row r="45" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
+      <c r="K45" s="42"/>
+    </row>
+    <row r="46" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
+      <c r="K46" s="42"/>
+    </row>
+    <row r="47" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42"/>
+      <c r="K47" s="42"/>
+    </row>
+    <row r="48" spans="2:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" s="35">
+        <v>1</v>
+      </c>
+      <c r="G48" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J48" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K48" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="39"/>
+      <c r="C49" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
+    </row>
+    <row r="50" spans="2:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="39"/>
+      <c r="C50" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53">
+        <v>1</v>
+      </c>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="35"/>
+    </row>
+    <row r="51" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="39"/>
+      <c r="C51" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53">
+        <v>2</v>
+      </c>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="35"/>
+    </row>
+    <row r="52" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="39"/>
+      <c r="C52" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="35">
+        <v>2</v>
+      </c>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="35"/>
+    </row>
+    <row r="53" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="39"/>
+      <c r="C53" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="35">
+        <v>3</v>
+      </c>
+      <c r="G53" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H53" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I53" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J53" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K53" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="39"/>
+      <c r="C54" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="35">
+        <v>2</v>
+      </c>
+      <c r="G54" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H54" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I54" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J54" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K54" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="41"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="42"/>
+      <c r="H55" s="42"/>
+      <c r="I55" s="42"/>
+      <c r="J55" s="42"/>
+      <c r="K55" s="42"/>
+    </row>
+    <row r="56" spans="2:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="D56" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F56" s="35">
+        <v>3</v>
+      </c>
+      <c r="G56" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H56" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I56" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J56" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K56" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="39"/>
+      <c r="C57" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D57" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="35">
+        <v>2</v>
+      </c>
+      <c r="G57" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I57" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J57" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K57" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="39"/>
+      <c r="C58" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D58" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="35">
+        <v>2</v>
+      </c>
+      <c r="G58" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H58" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I58" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J58" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K58" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="33"/>
+      <c r="C59" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="35">
+        <v>1</v>
+      </c>
+      <c r="G59" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H59" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I59" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J59" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K59" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="41"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="42"/>
+      <c r="H60" s="42"/>
+      <c r="I60" s="42"/>
+      <c r="J60" s="42"/>
+      <c r="K60" s="42"/>
+    </row>
+    <row r="61" spans="2:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="35">
+        <v>2</v>
+      </c>
+      <c r="G61" s="35">
+        <v>3</v>
+      </c>
+      <c r="H61" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I61" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J61" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K61" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="33"/>
+      <c r="C62" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62" s="35">
+        <v>2</v>
+      </c>
+      <c r="G62" s="35">
+        <v>2</v>
+      </c>
+      <c r="H62" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I62" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J62" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K62" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="33"/>
+      <c r="C63" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="35">
+        <v>1</v>
+      </c>
+      <c r="G63" s="35"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="35"/>
+    </row>
+    <row r="64" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="33"/>
+      <c r="C64" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="35">
+        <v>1</v>
+      </c>
+      <c r="G64" s="35"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="35"/>
+      <c r="J64" s="35"/>
+      <c r="K64" s="35"/>
+    </row>
+    <row r="65" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="33"/>
+      <c r="C65" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D65" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F65" s="35" t="e">
+        <f>SUM(#REF!,F54,F35,F30,F23)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G65" s="35" t="e">
+        <f>SUM(#REF!,G54,G30,G23,G35)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H65" s="35" t="e">
+        <f>SUM(#REF!,H54,H30,H23,H35)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I65" s="35" t="e">
+        <f>SUM(#REF!,I54,I30,I23,I35)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J65" s="35" t="e">
+        <f>SUM(#REF!,J54,J30,J23,J35)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K65" s="35" t="e">
+        <f>SUM(#REF!,K54,K30,K23,K35)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="33"/>
+      <c r="C66" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F66" s="35">
+        <f>SUM(F62,F57,F53,F33,F27,F7)</f>
+        <v>14</v>
+      </c>
+      <c r="G66" s="35">
+        <f>SUM(G62,G57,G53,G33,G27,G7)</f>
+        <v>2</v>
+      </c>
+      <c r="H66" s="35">
+        <f>SUM(H62,H57,H53,H33,H27,H7)</f>
+        <v>0</v>
+      </c>
+      <c r="I66" s="35">
+        <f>SUM(I62,I57,I53,I33,I27,I7)</f>
+        <v>0</v>
+      </c>
+      <c r="J66" s="35">
+        <f>SUM(J62,J57,J53,J33,J27,J7)</f>
+        <v>0</v>
+      </c>
+      <c r="K66" s="35">
+        <f>SUM(K62,K57,K53,K33,K27,K7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="33"/>
+      <c r="C67" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E67" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F67" s="35">
+        <f>SUM(F61,F56,F52,F32,F25,F6)</f>
+        <v>11.5</v>
+      </c>
+      <c r="G67" s="35"/>
+      <c r="H67" s="35"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="35"/>
+      <c r="K67" s="35"/>
+    </row>
+    <row r="68" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="33"/>
+      <c r="C68" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="F38" s="35">
-        <f>SUM(F29,F24,F19,F13,F8)</f>
-        <v>14</v>
-      </c>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
-      <c r="K38" s="35"/>
-    </row>
-    <row r="39" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="36"/>
-      <c r="C39" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" s="37">
-        <f t="shared" ref="F39:K39" si="1">SUM(F6:F34)</f>
-        <v>81</v>
-      </c>
-      <c r="G39" s="37">
-        <f t="shared" si="1"/>
+      <c r="E68" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F68" s="35">
+        <f>SUM(F58,F48,F34,F28,F8)</f>
+        <v>12</v>
+      </c>
+      <c r="G68" s="35"/>
+      <c r="H68" s="35"/>
+      <c r="I68" s="35"/>
+      <c r="J68" s="35"/>
+      <c r="K68" s="35"/>
+    </row>
+    <row r="69" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="36"/>
+      <c r="C69" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E69" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F69" s="37">
+        <f>SUM(F6:F62)</f>
+        <v>79</v>
+      </c>
+      <c r="G69" s="37">
+        <f>SUM(G6:G62)</f>
         <v>5</v>
       </c>
-      <c r="H39" s="37">
-        <f t="shared" si="1"/>
+      <c r="H69" s="37">
+        <f>SUM(H6:H62)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="37">
-        <f t="shared" si="1"/>
+      <c r="I69" s="37">
+        <f>SUM(I6:I62)</f>
         <v>0</v>
       </c>
-      <c r="J39" s="37">
-        <f t="shared" si="1"/>
+      <c r="J69" s="37">
+        <f>SUM(J6:J62)</f>
         <v>0</v>
       </c>
-      <c r="K39" s="37">
-        <f t="shared" si="1"/>
+      <c r="K69" s="37">
+        <f>SUM(K6:K62)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-    </row>
-    <row r="41" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-    </row>
-    <row r="42" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-    </row>
-    <row r="43" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-    </row>
-    <row r="44" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="24"/>
-    </row>
-    <row r="45" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="22"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-    </row>
-    <row r="46" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-    </row>
-    <row r="47" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-    </row>
-    <row r="48" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-    </row>
-    <row r="49" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-    </row>
-    <row r="50" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-    </row>
-    <row r="51" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-    </row>
-    <row r="52" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
+    <row r="70" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="11"/>
+    </row>
+    <row r="71" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11"/>
+    </row>
+    <row r="72" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="11"/>
+    </row>
+    <row r="73" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="11"/>
+      <c r="K73" s="11"/>
+    </row>
+    <row r="74" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="24"/>
+      <c r="I74" s="24"/>
+      <c r="J74" s="24"/>
+      <c r="K74" s="24"/>
+    </row>
+    <row r="75" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="22"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="11"/>
+      <c r="J75" s="11"/>
+      <c r="K75" s="11"/>
+    </row>
+    <row r="76" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="11"/>
+      <c r="K76" s="11"/>
+    </row>
+    <row r="77" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="11"/>
+      <c r="K77" s="11"/>
+    </row>
+    <row r="78" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="11"/>
+    </row>
+    <row r="79" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="11"/>
+    </row>
+    <row r="80" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="11"/>
+      <c r="K80" s="11"/>
+    </row>
+    <row r="81" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="11"/>
+      <c r="J81" s="11"/>
+      <c r="K81" s="11"/>
+    </row>
+    <row r="82" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="11"/>
+      <c r="J82" s="11"/>
+      <c r="K82" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="N6:U6"/>
   </mergeCells>
   <conditionalFormatting sqref="V5:W6 W27:W28 V29 X31:X65482 W30">
-    <cfRule type="cellIs" dxfId="15" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" stopIfTrue="1" operator="equal">
       <formula>"GREEN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="10" stopIfTrue="1" operator="equal">
       <formula>"YELLOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="11" stopIfTrue="1" operator="equal">
       <formula>"RED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:O15 T8:U15 S16:T16 L16:N16 L17:O26 T17:U26">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>L8&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3623,6 +4317,243 @@
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="A8:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="97" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="48"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="44"/>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="44"/>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="45"/>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="44"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="44"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="44"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="44"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="44"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="51"/>
+    </row>
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="51"/>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="51"/>
+    </row>
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 

</xml_diff>